<commit_message>
Updated the values in excel sheet
</commit_message>
<xml_diff>
--- a/Excels/Form101.xlsx
+++ b/Excels/Form101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advance Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7C7A904A-FE88-482B-A8CB-AEBE63DA7F63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D8C5C6FF-825B-4C32-91D2-C2D0301004C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6420" xr2:uid="{4A02A1B5-EAD1-40EB-8BB5-128BA5F420D9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>LastName</t>
   </si>
@@ -136,6 +136,27 @@
   </si>
   <si>
     <t>ValidityofClaim_dropdown</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test Address</t>
+  </si>
+  <si>
+    <t>Test OfcCity</t>
+  </si>
+  <si>
+    <t>Test Ofc State</t>
+  </si>
+  <si>
+    <t>Test Ofc Zip</t>
+  </si>
+  <si>
+    <t>Test Illenss</t>
+  </si>
+  <si>
+    <t>Eye</t>
   </si>
 </sst>
 </file>
@@ -490,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59596D1-F691-48F6-83E3-7933072A7EA3}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,6 +530,7 @@
     <col min="14" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -628,7 +650,58 @@
       <c r="J2" t="s">
         <v>17</v>
       </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2">
+        <v>123</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2">
+        <v>2345678909</v>
+      </c>
+      <c r="R2" s="1">
+        <v>40159</v>
+      </c>
+      <c r="S2" s="1">
+        <v>39428</v>
+      </c>
+      <c r="T2" s="1">
+        <v>40159</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
       <c r="V2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes made on Form101 and Test Execution classes, Created new driver class and package
</commit_message>
<xml_diff>
--- a/Excels/Form101.xlsx
+++ b/Excels/Form101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advance Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D8C5C6FF-825B-4C32-91D2-C2D0301004C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DCE45F01-4C92-4D9F-A2F5-9C2BA4FABD87}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6420" xr2:uid="{4A02A1B5-EAD1-40EB-8BB5-128BA5F420D9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>LastName</t>
   </si>
@@ -157,16 +157,84 @@
   </si>
   <si>
     <t>Eye</t>
+  </si>
+  <si>
+    <t>PartofBodyInjury</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>maritalStatus</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>NatureofInjury</t>
+  </si>
+  <si>
+    <t>Specific Injury - Laceration</t>
+  </si>
+  <si>
+    <t>WhatHappened</t>
+  </si>
+  <si>
+    <t>WhatObject</t>
+  </si>
+  <si>
+    <t>Test Object</t>
+  </si>
+  <si>
+    <t>Wasworkedemp</t>
+  </si>
+  <si>
+    <t>GrossEarnings</t>
+  </si>
+  <si>
+    <t>SubmitterEmail</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Doing</t>
+  </si>
+  <si>
+    <t>TestDoing</t>
+  </si>
+  <si>
+    <t>DOLastHire</t>
+  </si>
+  <si>
+    <t>CauseofInjury</t>
+  </si>
+  <si>
+    <t>Motor Vehicle - Vehicle Upset</t>
+  </si>
+  <si>
+    <t>Head - Eyes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,14 +257,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59596D1-F691-48F6-83E3-7933072A7EA3}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,17 +594,19 @@
     <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.26953125" customWidth="1"/>
     <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -562,64 +635,100 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>25</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>26</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>27</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>28</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>30</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>31</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>36</v>
       </c>
+      <c r="AE1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -648,55 +757,55 @@
         <v>90887</v>
       </c>
       <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>37</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>123</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>38</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>39</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>41</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>2345678909</v>
-      </c>
-      <c r="R2" s="1">
-        <v>40159</v>
-      </c>
-      <c r="S2" s="1">
-        <v>39428</v>
       </c>
       <c r="T2" s="1">
         <v>40159</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="1">
+        <v>39428</v>
+      </c>
+      <c r="V2" s="1">
+        <v>40159</v>
+      </c>
+      <c r="W2" t="s">
         <v>37</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>29</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>42</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>43</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>29</v>
       </c>
       <c r="AA2" t="s">
         <v>29</v>
@@ -704,8 +813,47 @@
       <c r="AB2" t="s">
         <v>29</v>
       </c>
+      <c r="AC2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>40159</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM2">
+        <v>2000</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AN2" r:id="rId1" xr:uid="{A09E18EF-EB10-496B-9FE6-EBB98FC3BB59}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes done in pageobject,executionpage and in smoke xml file.
</commit_message>
<xml_diff>
--- a/Excels/Form101.xlsx
+++ b/Excels/Form101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advance Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DCE45F01-4C92-4D9F-A2F5-9C2BA4FABD87}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{287A88CA-7D68-4D1B-92A5-C7F4ABA26F2F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6420" xr2:uid="{4A02A1B5-EAD1-40EB-8BB5-128BA5F420D9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>LastName</t>
   </si>
@@ -198,25 +198,40 @@
     <t>SubmitterEmail</t>
   </si>
   <si>
+    <t>Doing</t>
+  </si>
+  <si>
+    <t>TestDoing</t>
+  </si>
+  <si>
+    <t>DOLastHire</t>
+  </si>
+  <si>
+    <t>CauseofInjury</t>
+  </si>
+  <si>
+    <t>Motor Vehicle - Vehicle Upset</t>
+  </si>
+  <si>
+    <t>Head - Eyes</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test </t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
     <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>Doing</t>
-  </si>
-  <si>
-    <t>TestDoing</t>
-  </si>
-  <si>
-    <t>DOLastHire</t>
-  </si>
-  <si>
-    <t>CauseofInjury</t>
-  </si>
-  <si>
-    <t>Motor Vehicle - Vehicle Upset</t>
-  </si>
-  <si>
-    <t>Head - Eyes</t>
   </si>
 </sst>
 </file>
@@ -580,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59596D1-F691-48F6-83E3-7933072A7EA3}">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AL9" sqref="AL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -704,7 +719,7 @@
         <v>49</v>
       </c>
       <c r="AG1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AH1" t="s">
         <v>51</v>
@@ -713,10 +728,10 @@
         <v>52</v>
       </c>
       <c r="AJ1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AK1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL1" t="s">
         <v>54</v>
@@ -820,13 +835,13 @@
         <v>29</v>
       </c>
       <c r="AE2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AF2" t="s">
         <v>50</v>
       </c>
       <c r="AG2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH2" t="s">
         <v>17</v>
@@ -835,7 +850,7 @@
         <v>53</v>
       </c>
       <c r="AJ2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK2" s="1">
         <v>40159</v>
@@ -847,12 +862,134 @@
         <v>2000</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1">
+        <v>36841</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>90887</v>
+      </c>
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3">
+        <v>123</v>
+      </c>
+      <c r="O3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3">
+        <v>2345678909</v>
+      </c>
+      <c r="T3" s="1">
+        <v>40159</v>
+      </c>
+      <c r="U3" s="1">
+        <v>39428</v>
+      </c>
+      <c r="V3" s="1">
+        <v>40159</v>
+      </c>
+      <c r="W3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>40159</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM3">
+        <v>2000</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AN2" r:id="rId1" xr:uid="{A09E18EF-EB10-496B-9FE6-EBB98FC3BB59}"/>
+    <hyperlink ref="AN2" r:id="rId1" xr:uid="{DF29169C-7C89-4C86-A127-999A7358F04B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>